<commit_message>
Added three new tests to moran's I doc.
</commit_message>
<xml_diff>
--- a/method_comparison_table.xlsx
+++ b/method_comparison_table.xlsx
@@ -240,7 +240,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="56">
+  <cellStyleXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -251,6 +251,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -314,7 +322,7 @@
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="56">
+  <cellStyles count="64">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -342,6 +350,10 @@
     <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -369,6 +381,10 @@
     <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="9" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -702,7 +718,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -905,7 +921,7 @@
         <v>29</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>40</v>
@@ -952,7 +968,7 @@
         <v>28</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>29</v>
@@ -993,10 +1009,10 @@
         <v>30</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>28</v>
@@ -1005,7 +1021,7 @@
         <v>29</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="P6" s="4" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Added shuffled body site test for RDA.
</commit_message>
<xml_diff>
--- a/method_comparison_table.xlsx
+++ b/method_comparison_table.xlsx
@@ -718,7 +718,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1185,7 +1185,7 @@
         <v>37</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Updated table to include newest results for dbRDA.
</commit_message>
<xml_diff>
--- a/method_comparison_table.xlsx
+++ b/method_comparison_table.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="23080" yWindow="0" windowWidth="28120" windowHeight="26540" tabRatio="500"/>
   </bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="40">
   <si>
     <t>Whole body
 Body site</t>
@@ -140,29 +140,26 @@
 Key distance (distances) shuffled</t>
   </si>
   <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
-    <t>See note</t>
-  </si>
-  <si>
-    <t>Note: dbRDA is an ordination technique and does not have p-values. It produced ordination plots in accordance with the nature of the tests and appears to produce meaningful results.</t>
-  </si>
-  <si>
     <t>Citation</t>
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>Note: dbRDA is an ordination technique and does not have p-values. It produced ordination plots in accordance with the nature of the tests (i.e. positive/negative) and appears to produce meaningful results.</t>
+  </si>
+  <si>
+    <t>Meaningful</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -207,6 +204,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -240,7 +243,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="64">
+  <cellStyleXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -251,6 +254,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -322,7 +329,7 @@
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="64">
+  <cellStyles count="68">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -354,6 +361,8 @@
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -385,6 +394,8 @@
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="9" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -718,7 +729,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -774,7 +785,7 @@
         <v>10</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -824,7 +835,7 @@
         <v>30</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -874,7 +885,7 @@
         <v>30</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -924,7 +935,7 @@
         <v>28</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -974,7 +985,7 @@
         <v>29</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1024,7 +1035,7 @@
         <v>28</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1074,7 +1085,7 @@
         <v>30</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1097,7 +1108,7 @@
         <v>30</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>29</v>
@@ -1124,7 +1135,7 @@
         <v>30</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1174,7 +1185,7 @@
         <v>30</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1182,49 +1193,49 @@
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1268,8 +1279,15 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="45" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="20" max="16383" man="1"/>
+  </rowBreaks>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="16" max="1048575" man="1"/>
+  </colBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
dbRDA now has percent variability explained in the table. Also updated the legend a bit.
</commit_message>
<xml_diff>
--- a/method_comparison_table.xlsx
+++ b/method_comparison_table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="39">
   <si>
     <t>Whole body
 Body site</t>
@@ -92,9 +92,6 @@
     <t>Moran's I</t>
   </si>
   <si>
-    <t>dbRDA</t>
-  </si>
-  <si>
     <t>***   = significant at 0.01</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
   </si>
   <si>
     <t>Legend</t>
-  </si>
-  <si>
-    <t>N/A = test not performed</t>
   </si>
   <si>
     <t>****</t>
@@ -149,10 +143,13 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>Note: dbRDA is an ordination technique and does not have p-values. It produced ordination plots in accordance with the nature of the tests (i.e. positive/negative) and appears to produce meaningful results.</t>
-  </si>
-  <si>
-    <t>Meaningful</t>
+    <t>N/A = test not relevant</t>
+  </si>
+  <si>
+    <t>dbRDA*</t>
+  </si>
+  <si>
+    <t>* Note: dbRDA is an ordination technique and does not have p-values. It produces ordination plots in accordance with the nature of the tests (i.e. positive/negative controls) and appears to produce meaningful results based on previous analysis using principal coordinates analysis. The percent variability that is explained by each dbRDA model's constraining variable is included in the table instead of p-values.</t>
   </si>
 </sst>
 </file>
@@ -313,7 +310,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="9"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -327,6 +324,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="9" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="68">
@@ -729,7 +729,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -758,10 +758,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>5</v>
@@ -779,13 +779,13 @@
         <v>9</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -793,49 +793,49 @@
         <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -843,49 +843,49 @@
         <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -893,49 +893,49 @@
         <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -943,49 +943,49 @@
         <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -993,49 +993,49 @@
         <v>19</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1043,49 +1043,49 @@
         <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1093,49 +1093,49 @@
         <v>17</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1143,134 +1143,134 @@
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.27860000000000001</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3.2887E-2</v>
+      </c>
+      <c r="D10" s="6">
+        <v>6.9290000000000003E-3</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.33187</v>
+      </c>
+      <c r="F10" s="6">
+        <v>8.8813299999999998E-2</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>39</v>
+        <v>28</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.23280000000000001</v>
+      </c>
+      <c r="J10" s="6">
+        <v>9.5796600000000003E-3</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:1">

</xml_diff>

<commit_message>
Added PERMDISP to methods that are tested by workflow. Ready to start working on gradient analysis methods.
</commit_message>
<xml_diff>
--- a/method_comparison_table.xlsx
+++ b/method_comparison_table.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="23080" yWindow="0" windowWidth="28120" windowHeight="26540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="41">
   <si>
     <t>Whole body
 Body site</t>
@@ -146,10 +146,16 @@
     <t>N/A = test not relevant</t>
   </si>
   <si>
-    <t>dbRDA*</t>
-  </si>
-  <si>
     <t>* Note: dbRDA is an ordination technique and does not have p-values. It produces ordination plots in accordance with the nature of the tests (i.e. positive/negative controls) and appears to produce meaningful results based on previous analysis using principal coordinates analysis. The percent variability that is explained by each dbRDA model's constraining variable is included in the table instead of p-values.</t>
+  </si>
+  <si>
+    <t>PERMDISP</t>
+  </si>
+  <si>
+    <t>BEST</t>
+  </si>
+  <si>
+    <t>db-RDA*</t>
   </si>
 </sst>
 </file>
@@ -240,7 +246,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="68">
+  <cellStyleXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -251,6 +257,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -329,7 +339,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="68">
+  <cellStyles count="72">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -363,6 +373,8 @@
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -396,6 +408,8 @@
     <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="9" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -726,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1190,7 +1204,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B10" s="6">
         <v>0.27860000000000001</v>
@@ -1238,44 +1252,54 @@
         <v>35</v>
       </c>
     </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="12" spans="1:16">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" t="s">
-        <v>21</v>
+      <c r="A12" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>